<commit_message>
fix typo in cities_matrix
</commit_message>
<xml_diff>
--- a/resources/cities_matrix.xlsx
+++ b/resources/cities_matrix.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>Białystok</t>
   </si>
@@ -139,9 +139,6 @@
     <t>97.3</t>
   </si>
   <si>
-    <t>NowyTarg</t>
-  </si>
-  <si>
     <t>96.2</t>
   </si>
   <si>
@@ -247,12 +244,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -265,16 +268,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -291,13 +294,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -317,6 +320,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -516,12 +520,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -554,10 +558,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -805,12 +809,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1125,10 +1129,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2234,7 +2238,7 @@
     </row>
     <row r="16" ht="13.65" customHeight="1">
       <c r="A16" t="s" s="3">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4">
         <v>585</v>
@@ -2267,7 +2271,7 @@
         <v>163</v>
       </c>
       <c r="L16" t="s" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M16" s="4">
         <v>402</v>
@@ -2480,7 +2484,7 @@
         <v>374</v>
       </c>
       <c r="M19" t="s" s="3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N19" s="4">
         <v>271</v>
@@ -2527,7 +2531,7 @@
         <v>288</v>
       </c>
       <c r="D20" t="s" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="4">
         <v>470</v>
@@ -2545,7 +2549,7 @@
         <v>235</v>
       </c>
       <c r="J20" t="s" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K20" s="4">
         <v>240</v>
@@ -2572,7 +2576,7 @@
         <v>363</v>
       </c>
       <c r="S20" t="s" s="3">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T20" t="s" s="3">
         <v>31</v>
@@ -2624,7 +2628,7 @@
         <v>155</v>
       </c>
       <c r="K21" t="s" s="3">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L21" s="4">
         <v>172</v>
@@ -2699,7 +2703,7 @@
         <v>287</v>
       </c>
       <c r="J22" t="s" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K22" s="4">
         <v>143</v>
@@ -2855,13 +2859,13 @@
         <v>228</v>
       </c>
       <c r="H24" t="s" s="3">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I24" s="4">
         <v>200</v>
       </c>
       <c r="J24" t="s" s="3">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K24" s="4">
         <v>100</v>
@@ -2894,10 +2898,10 @@
         <v>159</v>
       </c>
       <c r="U24" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="V24" t="s" s="3">
         <v>52</v>
-      </c>
-      <c r="V24" t="s" s="3">
-        <v>53</v>
       </c>
       <c r="W24" s="4">
         <v>766</v>
@@ -3025,7 +3029,7 @@
         <v>190</v>
       </c>
       <c r="H26" t="s" s="3">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" s="4">
         <v>162</v>
@@ -3034,10 +3038,10 @@
         <v>111</v>
       </c>
       <c r="K26" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="L26" t="s" s="3">
         <v>55</v>
-      </c>
-      <c r="L26" t="s" s="3">
-        <v>56</v>
       </c>
       <c r="M26" s="4">
         <v>247</v>
@@ -3064,7 +3068,7 @@
         <v>192</v>
       </c>
       <c r="U26" t="s" s="3">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V26" s="4">
         <v>108</v>
@@ -3188,10 +3192,10 @@
         <v>503</v>
       </c>
       <c r="C28" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s" s="3">
         <v>58</v>
-      </c>
-      <c r="D28" t="s" s="3">
-        <v>59</v>
       </c>
       <c r="E28" s="4">
         <v>610</v>
@@ -3203,10 +3207,10 @@
         <v>121</v>
       </c>
       <c r="H28" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="I28" t="s" s="3">
         <v>60</v>
-      </c>
-      <c r="I28" t="s" s="3">
-        <v>61</v>
       </c>
       <c r="J28" s="4">
         <v>156</v>
@@ -3227,7 +3231,7 @@
         <v>594</v>
       </c>
       <c r="P28" t="s" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q28" s="4">
         <v>564</v>
@@ -3257,7 +3261,7 @@
         <v>397</v>
       </c>
       <c r="Z28" t="s" s="3">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA28" s="4">
         <v>309</v>
@@ -3413,7 +3417,7 @@
         <v>679</v>
       </c>
       <c r="P30" t="s" s="3">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q30" s="4">
         <v>621</v>
@@ -3500,7 +3504,7 @@
         <v>324</v>
       </c>
       <c r="M31" t="s" s="3">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N31" s="4">
         <v>398</v>
@@ -3568,10 +3572,10 @@
         <v>485</v>
       </c>
       <c r="C32" t="s" s="3">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s" s="3">
         <v>66</v>
-      </c>
-      <c r="D32" t="s" s="3">
-        <v>67</v>
       </c>
       <c r="E32" s="4">
         <v>596</v>
@@ -3637,13 +3641,13 @@
         <v>385</v>
       </c>
       <c r="Z32" t="s" s="3">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA32" s="4">
         <v>290</v>
       </c>
       <c r="AB32" t="s" s="3">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC32" s="4">
         <v>271</v>

</xml_diff>